<commit_message>
Made sheet2 the same as reader/sheet2 though the test needs rewriting: if both normal and iterable worksheets use read_dimension then separate tests for them are not required.
--HG--
branch : 1.8
</commit_message>
<xml_diff>
--- a/openpyxl/tests/test_data/genuine/empty.xlsx
+++ b/openpyxl/tests/test_data/genuine/empty.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="24800" windowHeight="12260" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="24800" windowHeight="12260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 - Text" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="Sheet3 - Formulas" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4 - Dates" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -33,8 +33,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,11 +82,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -374,15 +374,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -397,7 +396,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -405,49 +404,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="D1:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:AA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="4:11">
+    <row r="1" spans="4:27">
       <c r="D1">
         <v>1</v>
       </c>
       <c r="K1" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="2" spans="4:11">
+      <c r="AA1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="4:27">
       <c r="D2">
         <v>2</v>
       </c>
       <c r="K2" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="3" spans="4:11">
+      <c r="AA2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="4:27">
       <c r="D3">
         <v>3</v>
       </c>
       <c r="K3" s="1">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="4:11">
+      <c r="AA3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="4:27">
       <c r="D4">
         <v>4</v>
       </c>
       <c r="K4" s="1">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="4:11">
+      <c r="AA4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="4:27">
       <c r="D5">
         <v>5</v>
       </c>
@@ -457,211 +467,289 @@
       <c r="K5" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="4:11">
+      <c r="AA5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="4:27">
       <c r="D6">
         <v>6</v>
       </c>
       <c r="K6" s="1">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="7" spans="4:11">
+      <c r="AA6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="4:27">
       <c r="D7">
         <v>7</v>
       </c>
       <c r="K7" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="8" spans="4:11">
+      <c r="AA7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="4:27">
       <c r="D8">
         <v>8</v>
       </c>
       <c r="K8" s="1">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="9" spans="4:11">
+      <c r="AA8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="4:27">
       <c r="D9">
         <v>9</v>
       </c>
       <c r="K9" s="1">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="10" spans="4:11">
+      <c r="AA9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="4:27">
       <c r="D10">
         <v>10</v>
       </c>
       <c r="K10" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="4:11">
+      <c r="AA10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="4:27">
       <c r="D11">
         <v>11</v>
       </c>
       <c r="K11" s="1">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="12" spans="4:11">
+      <c r="AA11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="4:27">
       <c r="D12">
         <v>12</v>
       </c>
       <c r="K12" s="1">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="13" spans="4:11">
+      <c r="AA12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="4:27">
       <c r="D13">
         <v>13</v>
       </c>
       <c r="K13" s="1">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="14" spans="4:11">
+      <c r="AA13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="4:27">
       <c r="D14">
         <v>14</v>
       </c>
       <c r="K14" s="1">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="4:11">
+      <c r="AA14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="4:27">
       <c r="D15">
         <v>15</v>
       </c>
       <c r="K15" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="16" spans="4:11">
+      <c r="AA15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="4:27">
       <c r="D16">
         <v>16</v>
       </c>
       <c r="K16" s="1">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="17" spans="4:11">
+      <c r="AA16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="4:27">
       <c r="D17">
         <v>17</v>
       </c>
       <c r="K17" s="1">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="18" spans="4:11">
+      <c r="AA17">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27">
       <c r="D18">
         <v>18</v>
       </c>
       <c r="K18" s="1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="19" spans="4:11">
+      <c r="AA18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27">
       <c r="D19">
         <v>19</v>
       </c>
       <c r="K19" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="20" spans="4:11">
+      <c r="AA19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27">
       <c r="D20">
         <v>20</v>
       </c>
       <c r="K20" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="21" spans="4:11">
+      <c r="AA20">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27">
       <c r="D21">
         <v>21</v>
       </c>
       <c r="K21" s="1">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="22" spans="4:11">
+      <c r="AA21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27">
       <c r="D22">
         <v>22</v>
       </c>
       <c r="K22" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="23" spans="4:11">
+      <c r="AA22">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="4:27">
       <c r="D23">
         <v>23</v>
       </c>
       <c r="K23" s="1">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="24" spans="4:11">
+      <c r="AA23">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="4:27">
       <c r="D24">
         <v>24</v>
       </c>
       <c r="K24" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="25" spans="4:11">
+      <c r="AA24">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="4:27">
       <c r="D25">
         <v>25</v>
       </c>
       <c r="K25" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="26" spans="4:11">
+      <c r="AA25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="4:27">
       <c r="D26">
         <v>26</v>
       </c>
       <c r="K26" s="1">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="27" spans="4:11">
+      <c r="AA26">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="4:27">
       <c r="D27">
         <v>27</v>
       </c>
       <c r="K27" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="28" spans="4:11">
+      <c r="AA27">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="4:27">
       <c r="D28">
         <v>28</v>
       </c>
       <c r="K28" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="29" spans="4:11">
+      <c r="AA28">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="4:27">
       <c r="D29">
         <v>29</v>
       </c>
       <c r="K29" s="1">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="4:11">
+      <c r="AA29">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="4:27">
       <c r="D30">
         <v>30</v>
       </c>
       <c r="K30" s="1">
         <v>0.3</v>
+      </c>
+      <c r="AA30">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -669,15 +757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="4:4">
       <c r="D2">
@@ -689,7 +776,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -697,17 +784,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -721,9 +807,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>